<commit_message>
fix schedule Nikom, schedule to KRA, Edit title repay, edit menu bar
</commit_message>
<xml_diff>
--- a/app/storage/packages/loan/Repayment Schedule Nikom.xlsx
+++ b/app/storage/packages/loan/Repayment Schedule Nikom.xlsx
@@ -45,9 +45,6 @@
     <t>ហត្ថលេខាគណនេយ្យករ</t>
   </si>
   <si>
-    <t>ស្នាមមេដៃកូនបំណុល</t>
-  </si>
-  <si>
     <t>ផល រិទ្ធា</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>*ក្រោយពីបានពិនិត្យកិច្ចសន្យាខ្ចីប្រាក់ NK02 ខ្ញុំបាទ/នាងខ្ញុំ យល់ព្រមសងប្រាក់ តាមពេលវេលាដែលបានកំណត់ក្នុងតារាងនេះ។</t>
+  </si>
+  <si>
+    <t>ស្នាមមេដៃស្តាំអ្នកខ្ចី</t>
   </si>
 </sst>
 </file>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -248,9 +248,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -263,6 +260,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -273,9 +273,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -582,7 +579,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -598,7 +595,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -609,7 +606,7 @@
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -631,178 +628,178 @@
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="16"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>0</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="9">
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8">
         <v>0</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>0</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>0</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <f>D10+E10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>4000000</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>1</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="9">
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8">
         <v>0</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>10000000</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>2000</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <f>D11+E11</f>
         <v>10002000</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>4000000</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="A12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="A13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -811,28 +808,34 @@
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
-      <c r="F16" s="7" t="s">
-        <v>10</v>
+      <c r="F16" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="F7:G7"/>
@@ -847,12 +850,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
Fix repayment schedule for Nikom,  footer and header
</commit_message>
<xml_diff>
--- a/app/storage/packages/loan/Repayment Schedule Nikom.xlsx
+++ b/app/storage/packages/loan/Repayment Schedule Nikom.xlsx
@@ -75,9 +75,6 @@
     <t xml:space="preserve">អាសយដ្ឋាន៖ </t>
   </si>
   <si>
-    <t xml:space="preserve">រំលស់ការ៖ </t>
-  </si>
-  <si>
     <t xml:space="preserve">រំលស់ដើម៖ </t>
   </si>
   <si>
@@ -105,13 +102,16 @@
     <t>សាខា, អាសយដ្ឋាន៖, ទូរស័ព្ទ៖</t>
   </si>
   <si>
-    <t>*ករណីសងត្រឡប់មានការយីតយ៉ាវ ខ្ញុំបាទ/នាងខ្ញុំ សុខចិត្តលក់ទ្រព្យសម្បត្តិ ដើម្បីសងមកឱ្យស្ថាប័នគ្រប់ចំនួន។</t>
-  </si>
-  <si>
-    <t>*ក្រោយពីបានពិនិត្យកិច្ចសន្យាខ្ចីប្រាក់ NK02 ខ្ញុំបាទ/នាងខ្ញុំ យល់ព្រមសងប្រាក់ តាមពេលវេលាដែលបានកំណត់ក្នុងតារាងនេះ។</t>
-  </si>
-  <si>
-    <t>ស្នាមមេដៃស្តាំអ្នកខ្ចី</t>
+    <t>ស្នាមមេដៃស្តាំអ្នកបញ្ចាំ</t>
+  </si>
+  <si>
+    <t>*ក្រោយពីបានពិនិត្យកិច្ចសន្យាបញ្ចាំ NK02 ខ្ញុំបាទ/នាងខ្ញុំ យល់ព្រមសងប្រាក់ តាមពេលវេលាដែលបានកំណត់ក្នុងតារាងនេះ។</t>
+  </si>
+  <si>
+    <t>*ករណីសងត្រឡប់មានការយីតយ៉ាវ ខ្ញុំបាទ/នាងខ្ញុំ សុខចិត្តលក់ទ្រព្យសម្បត្តិ ដើម្បីសងមកក្រុមហ៊ុនគ្រប់ចំនួន។</t>
+  </si>
+  <si>
+    <t>Company</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +177,12 @@
       <color theme="1"/>
       <name val="Khmer OS Muol Light"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Khmer OS Muol Light"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -192,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -224,11 +230,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -260,19 +275,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -576,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="F8" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -594,163 +615,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="11" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>0</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9">
-        <f>D10+E10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <v>4000000</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
@@ -759,97 +765,121 @@
         <v>0</v>
       </c>
       <c r="D11" s="9">
-        <v>10000000</v>
+        <v>0</v>
       </c>
       <c r="E11" s="9">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="F11" s="9">
         <f>D11+E11</f>
-        <v>10002000</v>
+        <v>0</v>
       </c>
       <c r="G11" s="9">
         <v>4000000</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="8">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="9">
+        <v>10000000</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2000</v>
+      </c>
+      <c r="F12" s="9">
+        <f>D12+E12</f>
+        <v>10002000</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="F16" s="6" t="s">
+      <c r="F15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="F17" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="18" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>27</v>
+    <row r="19" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>